<commit_message>
update combined list using updated Panama Species list.
</commit_message>
<xml_diff>
--- a/tocheck/FloraPanamacodigosperdidos.xlsx
+++ b/tocheck/FloraPanamacodigosperdidos.xlsx
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="Y2" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="3">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="Y3" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="Y4" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="5">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="Y5" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="6">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="Y6" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="7">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="Y7" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="8">
@@ -1316,7 +1316,7 @@
         </is>
       </c>
       <c r="Y8" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="9">
@@ -1435,7 +1435,7 @@
         </is>
       </c>
       <c r="Y9" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="10">
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="Y10" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="11">
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="Y11" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
     <row r="12">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="Y12" s="2">
-        <v>45905</v>
+        <v>45909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>